<commit_message>
LMDI: Pasient.urbandistrict: La til samme beskrivelse som i organisasjon.urbandistrict (solves #25 closes #25) f0829722cc739fa3d76ec1b22c146e48a3f147a1
</commit_message>
<xml_diff>
--- a/currentbuild/StructureDefinition-legemiddel-classification.xlsx
+++ b/currentbuild/StructureDefinition-legemiddel-classification.xlsx
@@ -1270,7 +1270,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" hidden="true">
+    <row r="6">
       <c r="A6" t="s" s="2">
         <v>103</v>
       </c>
@@ -1375,12 +1375,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AK6">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>